<commit_message>
Analysis of previous data, new analysis
Ignoring high and low similarity columns technique
</commit_message>
<xml_diff>
--- a/GETComp/Análise - Modelo 003.xlsx
+++ b/GETComp/Análise - Modelo 003.xlsx
@@ -112,7 +112,7 @@
     <t>Número de indivíduos</t>
   </si>
   <si>
-    <t>c/ solução inicial que alcança aproximadamente 12%</t>
+    <t>C/ solução inicial que alcança aproximadamente 12%</t>
   </si>
 </sst>
 </file>
@@ -602,13 +602,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Ênfase1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -933,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1982,7 +1982,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1992,22 +1992,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>0.1</v>
       </c>
       <c r="B3" s="1">
@@ -2015,7 +2015,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>0.2</v>
       </c>
       <c r="B4" s="1">
@@ -2023,7 +2023,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>0.3</v>
       </c>
       <c r="B5" s="1">
@@ -2031,7 +2031,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>0.4</v>
       </c>
       <c r="B6" s="1">

</xml_diff>